<commit_message>
fix NA in Akhmatova
</commit_message>
<xml_diff>
--- a/data/Akhmatova_I4AbAb_AllData.xlsx
+++ b/data/Akhmatova_I4AbAb_AllData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ksenia/.yandex.disk/181445514/Yandex.Disk.localized/ПД_РАН/Dataset_I4_Akhmatova/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A42DEE4A-3237-AC48-9FA2-7282607050CB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4488A86B-A428-A347-914E-F2A886C39330}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="960" windowWidth="24540" windowHeight="14060" xr2:uid="{221F902B-571A-2745-B757-1F49300E1750}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="440">
   <si>
     <t>ID</t>
   </si>
@@ -1743,8 +1743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90004F7C-95E3-A04A-BE24-34A601B0C74A}">
   <dimension ref="A1:J377"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A351" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="E178" sqref="E178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -7431,6 +7431,9 @@
       <c r="D178" t="s">
         <v>8</v>
       </c>
+      <c r="E178" t="s">
+        <v>7</v>
+      </c>
       <c r="F178" t="s">
         <v>7</v>
       </c>

</xml_diff>